<commit_message>
working pom.xml and test data sorted
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testResults.xlsx
+++ b/src/main/resources/dataSheets/testResults.xlsx
@@ -11,12 +11,13 @@
     <sheet name="iPhone-6S " r:id="rId5" sheetId="3"/>
     <sheet name="iPhone-6S Plus " r:id="rId6" sheetId="4"/>
     <sheet name="iPhone-6 " r:id="rId7" sheetId="5"/>
+    <sheet name="Galaxy S7 " r:id="rId8" sheetId="6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="3">
   <si>
     <t>Test Parameters</t>
   </si>
@@ -189,4 +190,29 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.60546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="4.859375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>